<commit_message>
Cleanup. Make assembly instructions more clear with J7/J8
</commit_message>
<xml_diff>
--- a/Quantum BOM.xlsx
+++ b/Quantum BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cameron\git\TwillTech\3 Phase Driver\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\sirius.100stanford\Shared\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1009133E-8017-40DF-98DA-E6B2E9F94189}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA25F9C6-434F-4EB3-953B-507ED4A701AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="7395" windowWidth="29040" windowHeight="15840" xr2:uid="{215BDDDC-53A9-4F49-9BD1-06EF9DD1A63C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{215BDDDC-53A9-4F49-9BD1-06EF9DD1A63C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="170">
   <si>
     <t>CAPACITOR, 1µF 16V</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Single, 10BQ015</t>
   </si>
   <si>
-    <t>HEADERS_TEST, HDR2X3</t>
-  </si>
-  <si>
     <t>USB</t>
   </si>
   <si>
@@ -177,9 +174,6 @@
     <t>D2, D4, D7, D10</t>
   </si>
   <si>
-    <t>J7</t>
-  </si>
-  <si>
     <t>U7</t>
   </si>
   <si>
@@ -282,9 +276,6 @@
     <t>Ultiboard\SOD-123F</t>
   </si>
   <si>
-    <t>Ultiboard\MLX90363-Daughter-Mount</t>
-  </si>
-  <si>
     <t>Ultiboard\1051330011</t>
   </si>
   <si>
@@ -547,6 +538,9 @@
   </si>
   <si>
     <t>Do Not Insert</t>
+  </si>
+  <si>
+    <t>J7,J8</t>
   </si>
 </sst>
 </file>
@@ -910,8 +904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92DD560A-5DE4-4328-8B26-B27C7EFA3EE9}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,7 +914,7 @@
     <col min="2" max="2" width="44.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="41.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.85546875" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.7109375" customWidth="1"/>
     <col min="8" max="9" width="32.7109375" bestFit="1" customWidth="1"/>
@@ -929,34 +923,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F1" t="s">
         <v>150</v>
       </c>
-      <c r="B1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
+        <v>154</v>
+      </c>
+      <c r="H1" t="s">
         <v>151</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>152</v>
       </c>
-      <c r="E1" t="s">
-        <v>160</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>153</v>
-      </c>
-      <c r="G1" t="s">
-        <v>157</v>
-      </c>
-      <c r="H1" t="s">
-        <v>154</v>
-      </c>
-      <c r="I1" t="s">
-        <v>155</v>
-      </c>
-      <c r="J1" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -967,28 +961,28 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -996,31 +990,31 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1028,31 +1022,31 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1063,28 +1057,28 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1095,28 +1089,28 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1124,31 +1118,31 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1156,31 +1150,31 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1188,31 +1182,31 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1220,31 +1214,31 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1255,28 +1249,28 @@
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1284,31 +1278,31 @@
         <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1319,28 +1313,28 @@
         <v>0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1348,31 +1342,31 @@
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1380,31 +1374,31 @@
         <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1412,31 +1406,31 @@
         <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1447,28 +1441,28 @@
         <v>6</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1476,31 +1470,31 @@
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1511,28 +1505,28 @@
         <v>11</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1540,31 +1534,31 @@
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E20" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>164</v>
-      </c>
       <c r="H20" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1575,28 +1569,28 @@
         <v>10</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1604,31 +1598,31 @@
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1636,31 +1630,31 @@
         <v>2</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>48</v>
+        <v>169</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1668,31 +1662,31 @@
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1700,31 +1694,31 @@
         <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1735,28 +1729,28 @@
         <v>5</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F26" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="G26" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="I26" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1764,31 +1758,31 @@
         <v>1</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -1796,31 +1790,31 @@
         <v>1</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D28" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="G28" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -1828,31 +1822,31 @@
         <v>1</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -1860,31 +1854,31 @@
         <v>1</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -1892,31 +1886,31 @@
         <v>1</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -1924,31 +1918,31 @@
         <v>1</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -1956,31 +1950,31 @@
         <v>1</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -1988,31 +1982,31 @@
         <v>1</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E34" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -2023,28 +2017,28 @@
         <v>9</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -2052,31 +2046,31 @@
         <v>1</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -2087,7 +2081,7 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C38" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -2098,28 +2092,28 @@
         <v>8</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -2130,28 +2124,28 @@
         <v>7</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>